<commit_message>
Corrected binding site csv, started on BS analysis
</commit_message>
<xml_diff>
--- a/Binding_sites_numbering.xlsx
+++ b/Binding_sites_numbering.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jure\Documents\GitHub\gnomAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{132F5118-1420-4D3A-9AD4-51CE172A2DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7357137F-E0EC-42CB-ABE9-7AC32EFAFDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-45120" yWindow="-7680" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binding_sites_numbering" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="353">
   <si>
     <t>GABRA1_Alphafold</t>
   </si>
@@ -1184,9 +1184,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1266,6 +1263,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1550,7 +1550,7 @@
   <dimension ref="A1:E129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,1660 +1574,1902 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="23"/>
+      <c r="E2" s="22"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="23"/>
+      <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="23"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="23"/>
+      <c r="E8" s="22"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="23"/>
+      <c r="E9" s="22"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="23"/>
+      <c r="E10" s="22"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="23"/>
+      <c r="E11" s="22"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="23"/>
+      <c r="E12" s="22"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="23"/>
+      <c r="E13" s="22"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="23"/>
+      <c r="E14" s="22"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="23"/>
+      <c r="E15" s="22"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="23"/>
+      <c r="E16" s="22"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="23"/>
+      <c r="E17" s="22"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5" t="s">
+      <c r="A18" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="23"/>
+      <c r="E18" s="22"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="21" t="s">
+      <c r="A19" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="20" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="22" t="s">
+      <c r="A20" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="21" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="22" t="s">
+      <c r="A21" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="21" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="22" t="s">
+      <c r="A22" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="21" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="22" t="s">
+      <c r="A23" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="21" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="24" t="s">
+      <c r="A24" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="23" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="22" t="s">
+      <c r="A25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="21" t="s">
         <v>351</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="21" t="s">
         <v>352</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="20" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="22" t="s">
+      <c r="A26" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="21" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="22" t="s">
+      <c r="A27" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="21" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="22" t="s">
+      <c r="A28" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="21" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4" t="s">
+      <c r="A29" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="23"/>
+      <c r="E29" s="22"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4" t="s">
+      <c r="A30" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="23"/>
+      <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4" t="s">
+      <c r="A31" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="23"/>
+      <c r="E31" s="22"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4" t="s">
+      <c r="A32" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="23"/>
+      <c r="E32" s="22"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="5" t="s">
+      <c r="A33" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E33" s="23"/>
+      <c r="E33" s="22"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="6" t="s">
+      <c r="A34" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E34" s="23"/>
+      <c r="E34" s="22"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4" t="s">
+      <c r="A35" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="23"/>
+      <c r="E35" s="22"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E36" s="23"/>
+      <c r="E36" s="22"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="6" t="s">
+      <c r="A37" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E37" s="23"/>
+      <c r="E37" s="22"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4" t="s">
+      <c r="A38" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E38" s="23"/>
+      <c r="E38" s="22"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4" t="s">
+      <c r="A39" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E39" s="23"/>
+      <c r="E39" s="22"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4" t="s">
+      <c r="A40" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E40" s="23"/>
+      <c r="E40" s="22"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="3"/>
-      <c r="B41" s="5" t="s">
+      <c r="A41" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="E41" s="23"/>
+      <c r="E41" s="22"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="6" t="s">
+      <c r="A42" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E42" s="23"/>
+      <c r="E42" s="22"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="4" t="s">
+      <c r="A43" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E43" s="23"/>
+      <c r="E43" s="22"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="4" t="s">
+      <c r="A44" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E44" s="23"/>
+      <c r="E44" s="22"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="4" t="s">
+      <c r="A45" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="E45" s="23"/>
+      <c r="E45" s="22"/>
     </row>
     <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3"/>
-      <c r="B46" s="5" t="s">
+      <c r="A46" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E46" s="23"/>
+      <c r="E46" s="22"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="6" t="s">
+      <c r="A47" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E47" s="23"/>
+      <c r="E47" s="22"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-      <c r="B48" s="4" t="s">
+      <c r="A48" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E48" s="23"/>
+      <c r="E48" s="22"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="4" t="s">
+      <c r="A49" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="E49" s="23"/>
+      <c r="E49" s="22"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="4" t="s">
+      <c r="A50" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="E50" s="23"/>
+      <c r="E50" s="22"/>
     </row>
     <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="3"/>
-      <c r="B51" s="5" t="s">
+      <c r="A51" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E51" s="23"/>
+      <c r="E51" s="22"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="6" t="s">
+      <c r="A52" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="D52" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="E52" s="23"/>
+      <c r="E52" s="22"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="4" t="s">
+      <c r="A53" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="E53" s="23"/>
+      <c r="E53" s="22"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="B54" s="4" t="s">
+      <c r="A54" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E54" s="23"/>
+      <c r="E54" s="22"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="4" t="s">
+      <c r="A55" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E55" s="23"/>
+      <c r="E55" s="22"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-      <c r="B56" s="4" t="s">
+      <c r="A56" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E56" s="23"/>
+      <c r="E56" s="22"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="B57" s="4" t="s">
+      <c r="A57" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E57" s="23"/>
+      <c r="E57" s="22"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-      <c r="B58" s="4" t="s">
+      <c r="A58" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E58" s="23"/>
+      <c r="E58" s="22"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="B59" s="4" t="s">
+      <c r="A59" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E59" s="23"/>
+      <c r="E59" s="22"/>
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="3"/>
-      <c r="B60" s="5" t="s">
+      <c r="A60" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E60" s="23"/>
+      <c r="E60" s="22"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="B61" s="7" t="s">
+      <c r="A61" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="E61" s="23"/>
+      <c r="E61" s="22"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-      <c r="B62" s="8" t="s">
+      <c r="A62" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C62" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="D62" s="9" t="s">
+      <c r="D62" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E62" s="23"/>
+      <c r="E62" s="22"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
-      <c r="B63" s="8" t="s">
+      <c r="A63" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C63" s="9" t="s">
+      <c r="C63" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="D63" s="9" t="s">
+      <c r="D63" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="E63" s="23"/>
+      <c r="E63" s="22"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="3"/>
-      <c r="B64" s="8" t="s">
+      <c r="A64" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C64" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="D64" s="9" t="s">
+      <c r="D64" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E64" s="23"/>
+      <c r="E64" s="22"/>
     </row>
     <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="3"/>
-      <c r="B65" s="10" t="s">
+      <c r="A65" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="D65" s="11" t="s">
+      <c r="D65" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="E65" s="23"/>
+      <c r="E65" s="22"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="3"/>
-      <c r="B66" s="12" t="s">
+      <c r="A66" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C66" s="13" t="s">
+      <c r="C66" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="E66" s="23"/>
+      <c r="E66" s="22"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="3"/>
-      <c r="B67" s="14" t="s">
+      <c r="A67" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="C67" s="15" t="s">
+      <c r="C67" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="E67" s="23"/>
+      <c r="E67" s="22"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="3"/>
-      <c r="B68" s="14" t="s">
+      <c r="A68" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="C68" s="15" t="s">
+      <c r="C68" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="E68" s="23"/>
+      <c r="E68" s="22"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
-      <c r="B69" s="14" t="s">
+      <c r="A69" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="C69" s="15" t="s">
+      <c r="C69" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="D69" s="4" t="s">
+      <c r="D69" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E69" s="23"/>
+      <c r="E69" s="22"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
-      <c r="B70" s="14" t="s">
+      <c r="A70" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="C70" s="15" t="s">
+      <c r="C70" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="D70" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E70" s="23"/>
+      <c r="E70" s="22"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
-      <c r="B71" s="14" t="s">
+      <c r="A71" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C71" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="D71" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E71" s="23"/>
+      <c r="E71" s="22"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="3"/>
-      <c r="B72" s="14" t="s">
+      <c r="A72" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="C72" s="15" t="s">
+      <c r="C72" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="D72" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E72" s="23"/>
+      <c r="E72" s="22"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="3"/>
-      <c r="B73" s="14" t="s">
+      <c r="A73" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="C73" s="15" t="s">
+      <c r="C73" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="D73" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E73" s="23"/>
+      <c r="E73" s="22"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="3"/>
-      <c r="B74" s="14" t="s">
+      <c r="A74" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="C74" s="15" t="s">
+      <c r="C74" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D74" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E74" s="23"/>
+      <c r="E74" s="22"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-      <c r="B75" s="14" t="s">
+      <c r="A75" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="C75" s="15" t="s">
+      <c r="C75" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="D75" s="4" t="s">
+      <c r="D75" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="E75" s="23"/>
+      <c r="E75" s="22"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="3"/>
-      <c r="B76" s="14" t="s">
+      <c r="A76" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="C76" s="15" t="s">
+      <c r="C76" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D76" s="4" t="s">
+      <c r="D76" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E76" s="23"/>
+      <c r="E76" s="22"/>
     </row>
     <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="3"/>
-      <c r="B77" s="16" t="s">
+      <c r="A77" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="C77" s="17" t="s">
+      <c r="C77" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="E77" s="23"/>
+      <c r="E77" s="22"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B78" s="12" t="s">
+      <c r="B78" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="C78" s="13" t="s">
+      <c r="C78" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="D78" s="6" t="s">
+      <c r="D78" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="E78" s="23"/>
+      <c r="E78" s="22"/>
     </row>
     <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="3"/>
-      <c r="B79" s="16" t="s">
+      <c r="A79" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="C79" s="17" t="s">
+      <c r="C79" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="E79" s="23"/>
+      <c r="E79" s="22"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="3"/>
-      <c r="B80" s="12" t="s">
+      <c r="A80" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="C80" s="13" t="s">
+      <c r="C80" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="D80" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="E80" s="23"/>
+      <c r="E80" s="22"/>
     </row>
     <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="3"/>
-      <c r="B81" s="16" t="s">
+      <c r="A81" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="C81" s="17" t="s">
+      <c r="C81" s="16" t="s">
         <v>265</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="E81" s="23"/>
+      <c r="E81" s="22"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="3"/>
-      <c r="B82" s="12" t="s">
+      <c r="A82" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="C82" s="13" t="s">
+      <c r="C82" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="D82" s="6" t="s">
+      <c r="D82" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="E82" s="23"/>
+      <c r="E82" s="22"/>
     </row>
     <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="3"/>
-      <c r="B83" s="16" t="s">
+      <c r="A83" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="C83" s="17" t="s">
+      <c r="C83" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D83" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="E83" s="23"/>
+      <c r="E83" s="22"/>
     </row>
     <row r="84" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="3"/>
-      <c r="B84" s="18" t="s">
+      <c r="A84" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="C84" s="19" t="s">
+      <c r="C84" s="18" t="s">
         <v>268</v>
       </c>
-      <c r="D84" s="20" t="s">
+      <c r="D84" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="E84" s="23"/>
+      <c r="E84" s="22"/>
     </row>
     <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="3"/>
-      <c r="B85" s="18" t="s">
+      <c r="A85" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="C85" s="19" t="s">
+      <c r="C85" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="D85" s="20" t="s">
+      <c r="D85" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="E85" s="23"/>
+      <c r="E85" s="22"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="3"/>
-      <c r="B86" s="12" t="s">
+      <c r="A86" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="C86" s="13" t="s">
+      <c r="C86" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="D86" s="6" t="s">
+      <c r="D86" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="E86" s="23"/>
+      <c r="E86" s="22"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="3"/>
-      <c r="B87" s="14" t="s">
+      <c r="A87" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="C87" s="15" t="s">
+      <c r="C87" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="D87" s="4" t="s">
+      <c r="D87" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="E87" s="23"/>
+      <c r="E87" s="22"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="3"/>
-      <c r="B88" s="14" t="s">
+      <c r="A88" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="C88" s="15" t="s">
+      <c r="C88" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="D88" s="4" t="s">
+      <c r="D88" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="E88" s="23"/>
+      <c r="E88" s="22"/>
     </row>
     <row r="89" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="3"/>
-      <c r="B89" s="16" t="s">
+      <c r="A89" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="C89" s="17" t="s">
+      <c r="C89" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="D89" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="E89" s="23"/>
+      <c r="E89" s="22"/>
     </row>
     <row r="90" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="3"/>
-      <c r="B90" s="18" t="s">
+      <c r="A90" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="C90" s="19" t="s">
+      <c r="C90" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="D90" s="20" t="s">
+      <c r="D90" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="E90" s="23"/>
+      <c r="E90" s="22"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="3"/>
-      <c r="B91" s="12" t="s">
+      <c r="A91" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="C91" s="13" t="s">
+      <c r="C91" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="D91" s="6" t="s">
+      <c r="D91" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="E91" s="23"/>
+      <c r="E91" s="22"/>
     </row>
     <row r="92" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="3"/>
-      <c r="B92" s="16" t="s">
+      <c r="A92" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="C92" s="17" t="s">
+      <c r="C92" s="16" t="s">
         <v>276</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D92" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="E92" s="23"/>
+      <c r="E92" s="22"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="3"/>
-      <c r="B93" s="25" t="s">
+      <c r="A93" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" s="24" t="s">
         <v>350</v>
       </c>
-      <c r="C93" s="27" t="s">
+      <c r="C93" s="26" t="s">
         <v>277</v>
       </c>
-      <c r="D93" s="28" t="s">
+      <c r="D93" s="27" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="3"/>
-      <c r="B94" s="29" t="s">
+      <c r="A94" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="28" t="s">
         <v>240</v>
       </c>
-      <c r="C94" s="17" t="s">
+      <c r="C94" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="E94" s="30"/>
+      <c r="E94" s="29"/>
     </row>
     <row r="95" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="3"/>
-      <c r="B95" s="18" t="s">
+      <c r="A95" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="C95" s="19" t="s">
+      <c r="C95" s="18" t="s">
         <v>260</v>
       </c>
-      <c r="D95" s="20" t="s">
+      <c r="D95" s="19" t="s">
         <v>259</v>
       </c>
-      <c r="E95" s="23"/>
+      <c r="E95" s="22"/>
     </row>
     <row r="96" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B96" s="18" t="s">
+      <c r="B96" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="C96" s="19" t="s">
+      <c r="C96" s="18" t="s">
         <v>280</v>
       </c>
-      <c r="D96" s="20" t="s">
+      <c r="D96" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="E96" s="23"/>
+      <c r="E96" s="22"/>
     </row>
     <row r="97" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="3"/>
-      <c r="B97" s="18" t="s">
+      <c r="A97" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B97" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="C97" s="19" t="s">
+      <c r="C97" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="D97" s="20" t="s">
+      <c r="D97" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="E97" s="23"/>
+      <c r="E97" s="22"/>
     </row>
     <row r="98" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="3"/>
-      <c r="B98" s="18" t="s">
+      <c r="A98" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B98" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="C98" s="19" t="s">
+      <c r="C98" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="D98" s="20" t="s">
+      <c r="D98" s="19" t="s">
         <v>289</v>
       </c>
-      <c r="E98" s="23"/>
+      <c r="E98" s="22"/>
     </row>
     <row r="99" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="3"/>
-      <c r="B99" s="18" t="s">
+      <c r="A99" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B99" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="C99" s="19" t="s">
+      <c r="C99" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="D99" s="20" t="s">
+      <c r="D99" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="E99" s="23"/>
+      <c r="E99" s="22"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="3"/>
-      <c r="B100" s="12" t="s">
+      <c r="A100" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B100" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="C100" s="13" t="s">
+      <c r="C100" s="12" t="s">
         <v>296</v>
       </c>
-      <c r="D100" s="6" t="s">
+      <c r="D100" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="E100" s="23"/>
+      <c r="E100" s="22"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="3"/>
-      <c r="B101" s="14" t="s">
+      <c r="A101" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B101" s="13" t="s">
         <v>285</v>
       </c>
-      <c r="C101" s="15" t="s">
+      <c r="C101" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="D101" s="4" t="s">
+      <c r="D101" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="E101" s="23"/>
+      <c r="E101" s="22"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="3"/>
-      <c r="B102" s="14" t="s">
+      <c r="A102" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B102" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="C102" s="15" t="s">
+      <c r="C102" s="14" t="s">
         <v>236</v>
       </c>
-      <c r="D102" s="4" t="s">
+      <c r="D102" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="E102" s="23"/>
+      <c r="E102" s="22"/>
     </row>
     <row r="103" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="3"/>
-      <c r="B103" s="16" t="s">
+      <c r="A103" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B103" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="C103" s="17" t="s">
+      <c r="C103" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="D103" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="E103" s="23"/>
+      <c r="E103" s="22"/>
     </row>
     <row r="104" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="3"/>
-      <c r="B104" s="18" t="s">
+      <c r="A104" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B104" s="17" t="s">
         <v>287</v>
       </c>
-      <c r="C104" s="19" t="s">
+      <c r="C104" s="18" t="s">
         <v>299</v>
       </c>
-      <c r="D104" s="20" t="s">
+      <c r="D104" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="E104" s="23"/>
+      <c r="E104" s="22"/>
     </row>
     <row r="105" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="3"/>
-      <c r="B105" s="18" t="s">
+      <c r="A105" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B105" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="C105" s="19" t="s">
+      <c r="C105" s="18" t="s">
         <v>300</v>
       </c>
-      <c r="D105" s="20" t="s">
+      <c r="D105" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="E105" s="23"/>
+      <c r="E105" s="22"/>
     </row>
     <row r="106" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="3" t="s">
+      <c r="A106" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B106" s="19" t="s">
+      <c r="B106" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="C106" s="19" t="s">
+      <c r="C106" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="D106" s="19" t="s">
+      <c r="D106" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="E106" s="23"/>
+      <c r="E106" s="22"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="3"/>
-      <c r="B107" s="13" t="s">
+      <c r="A107" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B107" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="C107" s="13" t="s">
+      <c r="C107" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="D107" s="13" t="s">
+      <c r="D107" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="E107" s="23"/>
+      <c r="E107" s="22"/>
     </row>
     <row r="108" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="3"/>
-      <c r="B108" s="17" t="s">
+      <c r="A108" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B108" s="16" t="s">
         <v>330</v>
       </c>
-      <c r="C108" s="17" t="s">
+      <c r="C108" s="16" t="s">
         <v>345</v>
       </c>
-      <c r="D108" s="17" t="s">
+      <c r="D108" s="16" t="s">
         <v>337</v>
       </c>
-      <c r="E108" s="23"/>
+      <c r="E108" s="22"/>
     </row>
     <row r="109" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="3"/>
-      <c r="B109" s="19" t="s">
+      <c r="A109" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B109" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="C109" s="19" t="s">
+      <c r="C109" s="18" t="s">
         <v>346</v>
       </c>
-      <c r="D109" s="19" t="s">
+      <c r="D109" s="18" t="s">
         <v>338</v>
       </c>
-      <c r="E109" s="23"/>
+      <c r="E109" s="22"/>
     </row>
     <row r="110" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="3"/>
-      <c r="B110" s="19" t="s">
+      <c r="A110" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B110" s="18" t="s">
         <v>302</v>
       </c>
-      <c r="C110" s="19" t="s">
+      <c r="C110" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="D110" s="19" t="s">
+      <c r="D110" s="18" t="s">
         <v>339</v>
       </c>
-      <c r="E110" s="23"/>
+      <c r="E110" s="22"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="3"/>
-      <c r="B111" s="13" t="s">
+      <c r="A111" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B111" s="12" t="s">
         <v>332</v>
       </c>
-      <c r="C111" s="13" t="s">
+      <c r="C111" s="12" t="s">
         <v>347</v>
       </c>
-      <c r="D111" s="13" t="s">
+      <c r="D111" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="E111" s="23"/>
+      <c r="E111" s="22"/>
     </row>
     <row r="112" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="3"/>
-      <c r="B112" s="17" t="s">
+      <c r="A112" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B112" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="C112" s="17" t="s">
+      <c r="C112" s="16" t="s">
         <v>322</v>
       </c>
-      <c r="D112" s="17" t="s">
+      <c r="D112" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="E112" s="23"/>
+      <c r="E112" s="22"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="3"/>
-      <c r="B113" s="13" t="s">
+      <c r="A113" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B113" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="C113" s="13" t="s">
+      <c r="C113" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="D113" s="13" t="s">
+      <c r="D113" s="12" t="s">
         <v>341</v>
       </c>
-      <c r="E113" s="23"/>
+      <c r="E113" s="22"/>
     </row>
     <row r="114" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="3"/>
-      <c r="B114" s="17" t="s">
+      <c r="A114" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B114" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="C114" s="17" t="s">
+      <c r="C114" s="16" t="s">
         <v>323</v>
       </c>
-      <c r="D114" s="17" t="s">
+      <c r="D114" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="E114" s="23"/>
+      <c r="E114" s="22"/>
     </row>
     <row r="115" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="3"/>
-      <c r="B115" s="19" t="s">
+      <c r="A115" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B115" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="C115" s="19" t="s">
+      <c r="C115" s="18" t="s">
         <v>348</v>
       </c>
-      <c r="D115" s="19" t="s">
+      <c r="D115" s="18" t="s">
         <v>342</v>
       </c>
-      <c r="E115" s="23"/>
+      <c r="E115" s="22"/>
     </row>
     <row r="116" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="3"/>
-      <c r="B116" s="19" t="s">
+      <c r="A116" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B116" s="18" t="s">
         <v>335</v>
       </c>
-      <c r="C116" s="19" t="s">
+      <c r="C116" s="18" t="s">
         <v>349</v>
       </c>
-      <c r="D116" s="19" t="s">
+      <c r="D116" s="18" t="s">
         <v>343</v>
       </c>
-      <c r="E116" s="23"/>
+      <c r="E116" s="22"/>
     </row>
     <row r="117" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="3" t="s">
+      <c r="A117" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B117" s="19" t="s">
+      <c r="B117" s="18" t="s">
         <v>301</v>
       </c>
-      <c r="C117" s="19" t="s">
+      <c r="C117" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="D117" s="19" t="s">
+      <c r="D117" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="E117" s="23"/>
+      <c r="E117" s="22"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="3"/>
-      <c r="B118" s="13" t="s">
+      <c r="A118" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B118" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="C118" s="13" t="s">
+      <c r="C118" s="12" t="s">
         <v>320</v>
       </c>
-      <c r="D118" s="26" t="s">
+      <c r="D118" s="25" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="3"/>
-      <c r="B119" s="17" t="s">
+      <c r="A119" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B119" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="C119" s="17" t="s">
+      <c r="C119" s="16" t="s">
         <v>321</v>
       </c>
-      <c r="D119" s="31" t="s">
+      <c r="D119" s="30" t="s">
         <v>312</v>
       </c>
-      <c r="E119" s="23"/>
+      <c r="E119" s="22"/>
     </row>
     <row r="120" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="3"/>
-      <c r="B120" s="19" t="s">
+      <c r="A120" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B120" s="18" t="s">
         <v>304</v>
       </c>
-      <c r="C120" s="19" t="s">
+      <c r="C120" s="18" t="s">
         <v>322</v>
       </c>
-      <c r="D120" s="19" t="s">
+      <c r="D120" s="18" t="s">
         <v>313</v>
       </c>
-      <c r="E120" s="23"/>
+      <c r="E120" s="22"/>
     </row>
     <row r="121" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="3"/>
-      <c r="B121" s="19" t="s">
+      <c r="A121" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B121" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="C121" s="19" t="s">
+      <c r="C121" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="D121" s="19" t="s">
+      <c r="D121" s="18" t="s">
         <v>314</v>
       </c>
-      <c r="E121" s="23"/>
+      <c r="E121" s="22"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="3"/>
-      <c r="B122" s="13" t="s">
+      <c r="A122" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B122" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="C122" s="13" t="s">
+      <c r="C122" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="D122" s="13" t="s">
+      <c r="D122" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="E122" s="23"/>
+      <c r="E122" s="22"/>
     </row>
     <row r="123" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="3"/>
-      <c r="B123" s="17" t="s">
+      <c r="A123" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B123" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="C123" s="17" t="s">
+      <c r="C123" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="D123" s="17" t="s">
+      <c r="D123" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="E123" s="23"/>
+      <c r="E123" s="22"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="3"/>
-      <c r="B124" s="13" t="s">
+      <c r="A124" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B124" s="12" t="s">
         <v>307</v>
       </c>
-      <c r="C124" s="13" t="s">
+      <c r="C124" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="D124" s="13" t="s">
+      <c r="D124" s="12" t="s">
         <v>317</v>
       </c>
-      <c r="E124" s="23"/>
+      <c r="E124" s="22"/>
     </row>
     <row r="125" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="3"/>
-      <c r="B125" s="17" t="s">
+      <c r="A125" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B125" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="C125" s="17" t="s">
+      <c r="C125" s="16" t="s">
         <v>327</v>
       </c>
-      <c r="D125" s="17" t="s">
+      <c r="D125" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="E125" s="23"/>
+      <c r="E125" s="22"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="3"/>
-      <c r="B126" s="13" t="s">
+      <c r="A126" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B126" s="12" t="s">
         <v>309</v>
       </c>
-      <c r="C126" s="13" t="s">
+      <c r="C126" s="12" t="s">
         <v>329</v>
       </c>
-      <c r="D126" s="13" t="s">
+      <c r="D126" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="E126" s="23"/>
+      <c r="E126" s="22"/>
     </row>
     <row r="127" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="3"/>
-      <c r="B127" s="17" t="s">
+      <c r="A127" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B127" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="C127" s="17" t="s">
+      <c r="C127" s="16" t="s">
         <v>328</v>
       </c>
-      <c r="D127" s="17" t="s">
+      <c r="D127" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="E127" s="23"/>
+      <c r="E127" s="22"/>
     </row>
     <row r="128" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="3" t="s">
+      <c r="A128" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B128" s="19" t="s">
+      <c r="B128" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="C128" s="19" t="s">
+      <c r="C128" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="D128" s="19" t="s">
+      <c r="D128" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="E128" s="23"/>
+      <c r="E128" s="22"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="3"/>
+      <c r="A129" s="31" t="s">
+        <v>10</v>
+      </c>
       <c r="B129" s="1" t="s">
         <v>217</v>
       </c>
@@ -3237,18 +3479,9 @@
       <c r="D129" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E129" s="23"/>
+      <c r="E129" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A2:A33"/>
-    <mergeCell ref="A34:A77"/>
-    <mergeCell ref="A96:A105"/>
-    <mergeCell ref="A78:A95"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="A106:A116"/>
-    <mergeCell ref="A117:A127"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Right before cleaning up
</commit_message>
<xml_diff>
--- a/Binding_sites_numbering.xlsx
+++ b/Binding_sites_numbering.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jure\Documents\GitHub\gnomAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\gnomAD\gnomAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7357137F-E0EC-42CB-ABE9-7AC32EFAFDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCE549B-8EAD-4629-8AE6-51D22706FB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45120" yWindow="-7680" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binding_sites_numbering" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="362">
   <si>
     <t>GABRA1_Alphafold</t>
   </si>
@@ -1084,6 +1084,33 @@
   </si>
   <si>
     <t>G79</t>
+  </si>
+  <si>
+    <t>7 (Pore)</t>
+  </si>
+  <si>
+    <t>P280</t>
+  </si>
+  <si>
+    <t>T295</t>
+  </si>
+  <si>
+    <t>P253</t>
+  </si>
+  <si>
+    <t>L264</t>
+  </si>
+  <si>
+    <t>T268</t>
+  </si>
+  <si>
+    <t>P250</t>
+  </si>
+  <si>
+    <t>L261</t>
+  </si>
+  <si>
+    <t>T263</t>
   </si>
 </sst>
 </file>
@@ -1547,10 +1574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E129"/>
+  <dimension ref="A1:E137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="I127" sqref="I127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3481,6 +3508,126 @@
       </c>
       <c r="E129" s="22"/>
     </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="31" t="s">
+        <v>353</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="E130" s="22"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="31" t="s">
+        <v>353</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E131" s="22"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="31" t="s">
+        <v>353</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E132" s="22"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="31" t="s">
+        <v>353</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E133" s="22"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="31" t="s">
+        <v>353</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E134" s="22"/>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="31" t="s">
+        <v>353</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E135" s="22"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="31" t="s">
+        <v>353</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E136" s="22"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="31" t="s">
+        <v>353</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="E137" s="22"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>